<commit_message>
se aumento el tamaño del atributo SP
</commit_message>
<xml_diff>
--- a/web/files/import.xlsx
+++ b/web/files/import.xlsx
@@ -4146,9 +4146,9 @@
   <dimension ref="A1:AC147"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="D102" activeCellId="0" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -12651,10 +12651,10 @@
   </sheetPr>
   <dimension ref="A1:AB65"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="M51" activeCellId="0" sqref="M51"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B57" activeCellId="0" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -13538,7 +13538,7 @@
       <c r="AA14" s="0"/>
       <c r="AB14" s="0"/>
     </row>
-    <row r="15" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="31.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="22" t="n">
         <f aca="false">ROW()-1</f>
         <v>14</v>
@@ -16916,9 +16916,9 @@
   <dimension ref="A1:CP143"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+      <selection pane="bottomLeft" activeCell="C82" activeCellId="0" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -26199,8 +26199,8 @@
   </sheetPr>
   <dimension ref="A1:AA63"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A62" activeCellId="0" sqref="A62"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>